<commit_message>
refactor: make diffsearch result object and feature vector object
</commit_message>
<xml_diff>
--- a/src/main/resources/Recall/RecallResultCollection.xlsx
+++ b/src/main/resources/Recall/RecallResultCollection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bwedu-my.sharepoint.com/personal/paul_bredl_bwedu_de/Documents/Studium/Semester 7/BA/DiffSearch/src/main/resources/Recall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="856" documentId="8_{E1C1190B-3C9E-4A5F-AC21-6F7B60D85123}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BC20BE16-E6E0-4914-A4E6-EB6DA19C686F}"/>
+  <xr:revisionPtr revIDLastSave="863" documentId="8_{E1C1190B-3C9E-4A5F-AC21-6F7B60D85123}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{781F9059-9175-4B15-B500-C46E6F72384D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="10" xr2:uid="{25C56FF9-A069-44FD-B878-792FEE41DBD0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="3" xr2:uid="{25C56FF9-A069-44FD-B878-792FEE41DBD0}"/>
   </bookViews>
   <sheets>
     <sheet name="variing k" sheetId="3" r:id="rId1"/>
@@ -1130,25 +1130,7 @@
     <cellStyle name="Überschrift" xfId="1" builtinId="15"/>
     <cellStyle name="Überschrift 1" xfId="2" builtinId="16"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <b/>
@@ -1518,8 +1500,8 @@
   </sheetPr>
   <dimension ref="A1:P104"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14:K83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1930,17 +1912,17 @@
       <c r="G14" s="5">
         <v>9</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="80">
         <v>9</v>
       </c>
-      <c r="I14" s="12">
-        <v>1</v>
-      </c>
-      <c r="J14" s="13">
-        <v>1</v>
-      </c>
-      <c r="K14" s="61">
-        <v>6.6666666666666666E-2</v>
+      <c r="I14" s="85">
+        <v>1</v>
+      </c>
+      <c r="J14" s="86">
+        <v>1</v>
+      </c>
+      <c r="K14" s="81">
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="L14" s="5">
         <v>9</v>
@@ -1980,17 +1962,17 @@
       <c r="G15" s="5">
         <v>1160</v>
       </c>
-      <c r="H15" s="11">
-        <v>158</v>
-      </c>
-      <c r="I15" s="13">
-        <v>0.13620689655172413</v>
-      </c>
-      <c r="J15" s="13">
-        <v>0.13620689655172413</v>
-      </c>
-      <c r="K15" s="61">
-        <v>2.3255813953488372E-2</v>
+      <c r="H15" s="80">
+        <v>138</v>
+      </c>
+      <c r="I15" s="86">
+        <v>0.11896551724137931</v>
+      </c>
+      <c r="J15" s="86">
+        <v>0.11896551724137931</v>
+      </c>
+      <c r="K15" s="81">
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="L15" s="5">
         <v>1160</v>
@@ -2030,16 +2012,16 @@
       <c r="G16" s="5">
         <v>1554</v>
       </c>
-      <c r="H16" s="11">
-        <v>0</v>
-      </c>
-      <c r="I16" s="13">
-        <v>0</v>
-      </c>
-      <c r="J16" s="13">
-        <v>0</v>
-      </c>
-      <c r="K16" s="61">
+      <c r="H16" s="80">
+        <v>0</v>
+      </c>
+      <c r="I16" s="86">
+        <v>0</v>
+      </c>
+      <c r="J16" s="86">
+        <v>0</v>
+      </c>
+      <c r="K16" s="81">
         <v>0</v>
       </c>
       <c r="L16" s="5">
@@ -2080,16 +2062,16 @@
       <c r="G17" s="5">
         <v>28</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="80">
         <v>27</v>
       </c>
-      <c r="I17" s="13">
+      <c r="I17" s="86">
         <v>0.9642857142857143</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="86">
         <v>0.9642857142857143</v>
       </c>
-      <c r="K17" s="61">
+      <c r="K17" s="81">
         <v>1</v>
       </c>
       <c r="L17" s="5">
@@ -2130,17 +2112,17 @@
       <c r="G18" s="5">
         <v>553</v>
       </c>
-      <c r="H18" s="11">
-        <v>122</v>
-      </c>
-      <c r="I18" s="13">
-        <v>0.22061482820976491</v>
-      </c>
-      <c r="J18" s="13">
-        <v>0.22061482820976491</v>
-      </c>
-      <c r="K18" s="61">
-        <v>6.6666666666666666E-2</v>
+      <c r="H18" s="80">
+        <v>8</v>
+      </c>
+      <c r="I18" s="86">
+        <v>1.4466546112115732E-2</v>
+      </c>
+      <c r="J18" s="86">
+        <v>1.4466546112115732E-2</v>
+      </c>
+      <c r="K18" s="81">
+        <v>0.25</v>
       </c>
       <c r="L18" s="5">
         <v>553</v>
@@ -2180,16 +2162,16 @@
       <c r="G19" s="5">
         <v>431</v>
       </c>
-      <c r="H19" s="11">
-        <v>28</v>
-      </c>
-      <c r="I19" s="13">
-        <v>6.4965197215777259E-2</v>
-      </c>
-      <c r="J19" s="13">
-        <v>6.4965197215777259E-2</v>
-      </c>
-      <c r="K19" s="61">
+      <c r="H19" s="80">
+        <v>31</v>
+      </c>
+      <c r="I19" s="86">
+        <v>7.1925754060324823E-2</v>
+      </c>
+      <c r="J19" s="86">
+        <v>7.1925754060324823E-2</v>
+      </c>
+      <c r="K19" s="81">
         <v>0.5</v>
       </c>
       <c r="L19" s="5">
@@ -2230,16 +2212,16 @@
       <c r="G20" s="5">
         <v>97768</v>
       </c>
-      <c r="H20" s="11">
+      <c r="H20" s="80">
         <v>256</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="86">
         <v>2.6184436625480731E-3</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="86">
         <v>5.1200000000000002E-2</v>
       </c>
-      <c r="K20" s="61">
+      <c r="K20" s="81">
         <v>1</v>
       </c>
       <c r="L20" s="5">
@@ -2280,17 +2262,17 @@
       <c r="G21" s="5">
         <v>28</v>
       </c>
-      <c r="H21" s="11">
-        <v>23</v>
-      </c>
-      <c r="I21" s="13">
-        <v>0.8214285714285714</v>
-      </c>
-      <c r="J21" s="13">
-        <v>0.8214285714285714</v>
-      </c>
-      <c r="K21" s="61">
-        <v>0.33333333333333331</v>
+      <c r="H21" s="80">
+        <v>8</v>
+      </c>
+      <c r="I21" s="86">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="J21" s="86">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="K21" s="81">
+        <v>0.5</v>
       </c>
       <c r="L21" s="5">
         <v>28</v>
@@ -2330,17 +2312,17 @@
       <c r="G22" s="5">
         <v>1554</v>
       </c>
-      <c r="H22" s="11">
-        <v>546</v>
-      </c>
-      <c r="I22" s="13">
-        <v>0.35135135135135137</v>
-      </c>
-      <c r="J22" s="13">
-        <v>0.35135135135135137</v>
-      </c>
-      <c r="K22" s="61">
-        <v>0.25</v>
+      <c r="H22" s="80">
+        <v>114</v>
+      </c>
+      <c r="I22" s="86">
+        <v>7.3359073359073365E-2</v>
+      </c>
+      <c r="J22" s="86">
+        <v>7.3359073359073365E-2</v>
+      </c>
+      <c r="K22" s="81">
+        <v>0.33333333333333331</v>
       </c>
       <c r="L22" s="5">
         <v>1554</v>
@@ -2380,17 +2362,17 @@
       <c r="G23" s="5">
         <v>123</v>
       </c>
-      <c r="H23" s="11">
-        <v>23</v>
-      </c>
-      <c r="I23" s="13">
-        <v>0.18699186991869918</v>
-      </c>
-      <c r="J23" s="13">
-        <v>0.18699186991869918</v>
-      </c>
-      <c r="K23" s="61">
-        <v>3.1250000000000002E-3</v>
+      <c r="H23" s="80">
+        <v>8</v>
+      </c>
+      <c r="I23" s="86">
+        <v>6.5040650406504072E-2</v>
+      </c>
+      <c r="J23" s="86">
+        <v>6.5040650406504072E-2</v>
+      </c>
+      <c r="K23" s="81">
+        <v>4.807692307692308E-3</v>
       </c>
       <c r="L23" s="5">
         <v>123</v>
@@ -2430,17 +2412,17 @@
       <c r="G24" s="5">
         <v>40485</v>
       </c>
-      <c r="H24" s="11">
-        <v>462</v>
-      </c>
-      <c r="I24" s="13">
-        <v>1.1411633938495739E-2</v>
-      </c>
-      <c r="J24" s="13">
-        <v>9.2399999999999996E-2</v>
-      </c>
-      <c r="K24" s="61">
-        <v>1.9607843137254902E-3</v>
+      <c r="H24" s="80">
+        <v>114</v>
+      </c>
+      <c r="I24" s="86">
+        <v>2.8158577250833642E-3</v>
+      </c>
+      <c r="J24" s="86">
+        <v>2.2800000000000001E-2</v>
+      </c>
+      <c r="K24" s="81">
+        <v>1.7452006980802793E-3</v>
       </c>
       <c r="L24" s="5">
         <v>40485</v>
@@ -2480,17 +2462,17 @@
       <c r="G25" s="5">
         <v>388</v>
       </c>
-      <c r="H25" s="11">
-        <v>223</v>
-      </c>
-      <c r="I25" s="13">
-        <v>0.57474226804123707</v>
-      </c>
-      <c r="J25" s="13">
-        <v>0.57474226804123707</v>
-      </c>
-      <c r="K25" s="61">
-        <v>0.125</v>
+      <c r="H25" s="80">
+        <v>212</v>
+      </c>
+      <c r="I25" s="86">
+        <v>0.54639175257731953</v>
+      </c>
+      <c r="J25" s="86">
+        <v>0.54639175257731953</v>
+      </c>
+      <c r="K25" s="81">
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="L25" s="5">
         <v>388</v>
@@ -2530,16 +2512,16 @@
       <c r="G26" s="5">
         <v>577</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H26" s="80">
         <v>103</v>
       </c>
-      <c r="I26" s="13">
+      <c r="I26" s="86">
         <v>0.17850953206239167</v>
       </c>
-      <c r="J26" s="13">
+      <c r="J26" s="86">
         <v>0.17850953206239167</v>
       </c>
-      <c r="K26" s="61">
+      <c r="K26" s="81">
         <v>1</v>
       </c>
       <c r="L26" s="5">
@@ -2580,16 +2562,16 @@
       <c r="G27" s="5">
         <v>142</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H27" s="80">
         <v>123</v>
       </c>
-      <c r="I27" s="13">
+      <c r="I27" s="86">
         <v>0.86619718309859151</v>
       </c>
-      <c r="J27" s="13">
+      <c r="J27" s="86">
         <v>0.86619718309859151</v>
       </c>
-      <c r="K27" s="61">
+      <c r="K27" s="81">
         <v>0.14285714285714285</v>
       </c>
       <c r="L27" s="5">
@@ -2630,16 +2612,16 @@
       <c r="G28" s="5">
         <v>158355</v>
       </c>
-      <c r="H28" s="11">
+      <c r="H28" s="80">
         <v>4586</v>
       </c>
-      <c r="I28" s="13">
+      <c r="I28" s="86">
         <v>2.896024754507278E-2</v>
       </c>
-      <c r="J28" s="13">
+      <c r="J28" s="86">
         <v>0.91720000000000002</v>
       </c>
-      <c r="K28" s="61">
+      <c r="K28" s="81">
         <v>1</v>
       </c>
       <c r="L28" s="5">
@@ -2680,16 +2662,16 @@
       <c r="G29" s="5">
         <v>323</v>
       </c>
-      <c r="H29" s="11">
-        <v>192</v>
-      </c>
-      <c r="I29" s="13">
-        <v>0.59442724458204332</v>
-      </c>
-      <c r="J29" s="13">
-        <v>0.59442724458204332</v>
-      </c>
-      <c r="K29" s="61">
+      <c r="H29" s="80">
+        <v>191</v>
+      </c>
+      <c r="I29" s="86">
+        <v>0.59133126934984526</v>
+      </c>
+      <c r="J29" s="86">
+        <v>0.59133126934984526</v>
+      </c>
+      <c r="K29" s="81">
         <v>1</v>
       </c>
       <c r="L29" s="5">
@@ -2730,17 +2712,17 @@
       <c r="G30" s="5">
         <v>5</v>
       </c>
-      <c r="H30" s="11">
-        <v>1</v>
-      </c>
-      <c r="I30" s="13">
+      <c r="H30" s="80">
+        <v>1</v>
+      </c>
+      <c r="I30" s="86">
         <v>0.2</v>
       </c>
-      <c r="J30" s="13">
+      <c r="J30" s="86">
         <v>0.2</v>
       </c>
-      <c r="K30" s="61">
-        <v>7.6923076923076927E-2</v>
+      <c r="K30" s="81">
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="L30" s="5">
         <v>5</v>
@@ -2780,16 +2762,16 @@
       <c r="G31" s="5">
         <v>13</v>
       </c>
-      <c r="H31" s="11">
+      <c r="H31" s="80">
         <v>8</v>
       </c>
-      <c r="I31" s="13">
+      <c r="I31" s="86">
         <v>0.61538461538461542</v>
       </c>
-      <c r="J31" s="13">
+      <c r="J31" s="86">
         <v>0.61538461538461542</v>
       </c>
-      <c r="K31" s="61">
+      <c r="K31" s="81">
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L31" s="5">
@@ -2830,17 +2812,17 @@
       <c r="G32" s="5">
         <v>158</v>
       </c>
-      <c r="H32" s="11">
-        <v>86</v>
-      </c>
-      <c r="I32" s="13">
-        <v>0.54430379746835444</v>
-      </c>
-      <c r="J32" s="13">
-        <v>0.54430379746835444</v>
-      </c>
-      <c r="K32" s="61">
-        <v>1</v>
+      <c r="H32" s="80">
+        <v>87</v>
+      </c>
+      <c r="I32" s="86">
+        <v>0.55063291139240511</v>
+      </c>
+      <c r="J32" s="86">
+        <v>0.55063291139240511</v>
+      </c>
+      <c r="K32" s="81">
+        <v>0.5</v>
       </c>
       <c r="L32" s="5">
         <v>158</v>
@@ -2880,16 +2862,16 @@
       <c r="G33" s="5">
         <v>247</v>
       </c>
-      <c r="H33" s="11">
-        <v>1</v>
-      </c>
-      <c r="I33" s="13">
+      <c r="H33" s="80">
+        <v>1</v>
+      </c>
+      <c r="I33" s="86">
         <v>4.048582995951417E-3</v>
       </c>
-      <c r="J33" s="13">
+      <c r="J33" s="86">
         <v>4.048582995951417E-3</v>
       </c>
-      <c r="K33" s="61">
+      <c r="K33" s="81">
         <v>1</v>
       </c>
       <c r="L33" s="5">
@@ -2930,17 +2912,17 @@
       <c r="G34" s="5">
         <v>83</v>
       </c>
-      <c r="H34" s="11">
+      <c r="H34" s="80">
         <v>72</v>
       </c>
-      <c r="I34" s="13">
+      <c r="I34" s="86">
         <v>0.86746987951807231</v>
       </c>
-      <c r="J34" s="13">
+      <c r="J34" s="86">
         <v>0.86746987951807231</v>
       </c>
-      <c r="K34" s="61">
-        <v>0.125</v>
+      <c r="K34" s="81">
+        <v>0.16666666666666666</v>
       </c>
       <c r="L34" s="5">
         <v>83</v>
@@ -2980,16 +2962,16 @@
       <c r="G35" s="5">
         <v>16</v>
       </c>
-      <c r="H35" s="11">
+      <c r="H35" s="80">
         <v>16</v>
       </c>
-      <c r="I35" s="13">
-        <v>1</v>
-      </c>
-      <c r="J35" s="13">
-        <v>1</v>
-      </c>
-      <c r="K35" s="61">
+      <c r="I35" s="86">
+        <v>1</v>
+      </c>
+      <c r="J35" s="86">
+        <v>1</v>
+      </c>
+      <c r="K35" s="81">
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="L35" s="5">
@@ -3030,17 +3012,17 @@
       <c r="G36" s="5">
         <v>24</v>
       </c>
-      <c r="H36" s="11">
-        <v>16</v>
-      </c>
-      <c r="I36" s="13">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="J36" s="13">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="K36" s="61">
-        <v>2.7777777777777776E-2</v>
+      <c r="H36" s="80">
+        <v>0</v>
+      </c>
+      <c r="I36" s="86">
+        <v>0</v>
+      </c>
+      <c r="J36" s="86">
+        <v>0</v>
+      </c>
+      <c r="K36" s="81">
+        <v>0</v>
       </c>
       <c r="L36" s="5">
         <v>24</v>
@@ -3080,17 +3062,17 @@
       <c r="G37" s="5">
         <v>35</v>
       </c>
-      <c r="H37" s="11">
+      <c r="H37" s="80">
         <v>30</v>
       </c>
-      <c r="I37" s="13">
+      <c r="I37" s="86">
         <v>0.8571428571428571</v>
       </c>
-      <c r="J37" s="13">
+      <c r="J37" s="86">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K37" s="61">
-        <v>1.0869565217391304E-2</v>
+      <c r="K37" s="81">
+        <v>1.2658227848101266E-2</v>
       </c>
       <c r="L37" s="5">
         <v>35</v>
@@ -3130,16 +3112,16 @@
       <c r="G38" s="5">
         <v>88</v>
       </c>
-      <c r="H38" s="11">
-        <v>0</v>
-      </c>
-      <c r="I38" s="13">
-        <v>0</v>
-      </c>
-      <c r="J38" s="13">
-        <v>0</v>
-      </c>
-      <c r="K38" s="61">
+      <c r="H38" s="80">
+        <v>0</v>
+      </c>
+      <c r="I38" s="86">
+        <v>0</v>
+      </c>
+      <c r="J38" s="86">
+        <v>0</v>
+      </c>
+      <c r="K38" s="81">
         <v>0</v>
       </c>
       <c r="L38" s="5">
@@ -3180,17 +3162,17 @@
       <c r="G39" s="5">
         <v>80</v>
       </c>
-      <c r="H39" s="11">
+      <c r="H39" s="80">
         <v>49</v>
       </c>
-      <c r="I39" s="13">
+      <c r="I39" s="86">
         <v>0.61250000000000004</v>
       </c>
-      <c r="J39" s="13">
+      <c r="J39" s="86">
         <v>0.61250000000000004</v>
       </c>
-      <c r="K39" s="61">
-        <v>1</v>
+      <c r="K39" s="81">
+        <v>0.5</v>
       </c>
       <c r="L39" s="5">
         <v>80</v>
@@ -3230,16 +3212,16 @@
       <c r="G40" s="5">
         <v>66</v>
       </c>
-      <c r="H40" s="11">
+      <c r="H40" s="80">
         <v>53</v>
       </c>
-      <c r="I40" s="13">
+      <c r="I40" s="86">
         <v>0.80303030303030298</v>
       </c>
-      <c r="J40" s="13">
+      <c r="J40" s="86">
         <v>0.80303030303030298</v>
       </c>
-      <c r="K40" s="61">
+      <c r="K40" s="81">
         <v>0.2</v>
       </c>
       <c r="L40" s="5">
@@ -3280,17 +3262,17 @@
       <c r="G41" s="5">
         <v>15</v>
       </c>
-      <c r="H41" s="11">
-        <v>2</v>
-      </c>
-      <c r="I41" s="13">
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="J41" s="13">
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="K41" s="61">
-        <v>4.3478260869565218E-3</v>
+      <c r="H41" s="80">
+        <v>0</v>
+      </c>
+      <c r="I41" s="86">
+        <v>0</v>
+      </c>
+      <c r="J41" s="86">
+        <v>0</v>
+      </c>
+      <c r="K41" s="81">
+        <v>0</v>
       </c>
       <c r="L41" s="5">
         <v>15</v>
@@ -3330,17 +3312,17 @@
       <c r="G42" s="5">
         <v>332</v>
       </c>
-      <c r="H42" s="11">
+      <c r="H42" s="80">
         <v>11</v>
       </c>
-      <c r="I42" s="13">
+      <c r="I42" s="86">
         <v>3.313253012048193E-2</v>
       </c>
-      <c r="J42" s="13">
+      <c r="J42" s="86">
         <v>3.313253012048193E-2</v>
       </c>
-      <c r="K42" s="61">
-        <v>0.14285714285714285</v>
+      <c r="K42" s="81">
+        <v>1</v>
       </c>
       <c r="L42" s="5">
         <v>332</v>
@@ -3380,17 +3362,17 @@
       <c r="G43" s="5">
         <v>39</v>
       </c>
-      <c r="H43" s="11">
+      <c r="H43" s="80">
         <v>2</v>
       </c>
-      <c r="I43" s="13">
+      <c r="I43" s="86">
         <v>5.128205128205128E-2</v>
       </c>
-      <c r="J43" s="13">
+      <c r="J43" s="86">
         <v>5.128205128205128E-2</v>
       </c>
-      <c r="K43" s="61">
-        <v>8.9525514771709937E-4</v>
+      <c r="K43" s="81">
+        <v>5.461496450027307E-4</v>
       </c>
       <c r="L43" s="5">
         <v>39</v>
@@ -3430,17 +3412,17 @@
       <c r="G44" s="5">
         <v>1</v>
       </c>
-      <c r="H44" s="11">
-        <v>1</v>
-      </c>
-      <c r="I44" s="13">
-        <v>1</v>
-      </c>
-      <c r="J44" s="13">
-        <v>1</v>
-      </c>
-      <c r="K44" s="61">
-        <v>0.16666666666666666</v>
+      <c r="H44" s="80">
+        <v>1</v>
+      </c>
+      <c r="I44" s="86">
+        <v>1</v>
+      </c>
+      <c r="J44" s="86">
+        <v>1</v>
+      </c>
+      <c r="K44" s="81">
+        <v>0.1</v>
       </c>
       <c r="L44" s="5">
         <v>1</v>
@@ -3480,17 +3462,17 @@
       <c r="G45" s="5">
         <v>431</v>
       </c>
-      <c r="H45" s="11">
-        <v>331</v>
-      </c>
-      <c r="I45" s="13">
-        <v>0.76798143851508116</v>
-      </c>
-      <c r="J45" s="13">
-        <v>0.76798143851508116</v>
-      </c>
-      <c r="K45" s="61">
-        <v>0.05</v>
+      <c r="H45" s="80">
+        <v>322</v>
+      </c>
+      <c r="I45" s="86">
+        <v>0.74709976798143851</v>
+      </c>
+      <c r="J45" s="86">
+        <v>0.74709976798143851</v>
+      </c>
+      <c r="K45" s="81">
+        <v>3.8461538461538464E-2</v>
       </c>
       <c r="L45" s="5">
         <v>431</v>
@@ -3530,17 +3512,17 @@
       <c r="G46" s="5">
         <v>40</v>
       </c>
-      <c r="H46" s="11">
+      <c r="H46" s="80">
         <v>40</v>
       </c>
-      <c r="I46" s="13">
-        <v>1</v>
-      </c>
-      <c r="J46" s="13">
-        <v>1</v>
-      </c>
-      <c r="K46" s="61">
-        <v>2.6315789473684209E-2</v>
+      <c r="I46" s="86">
+        <v>1</v>
+      </c>
+      <c r="J46" s="86">
+        <v>1</v>
+      </c>
+      <c r="K46" s="81">
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="L46" s="5">
         <v>40</v>
@@ -3580,17 +3562,17 @@
       <c r="G47" s="5">
         <v>40</v>
       </c>
-      <c r="H47" s="11">
+      <c r="H47" s="80">
         <v>40</v>
       </c>
-      <c r="I47" s="13">
-        <v>1</v>
-      </c>
-      <c r="J47" s="13">
-        <v>1</v>
-      </c>
-      <c r="K47" s="61">
-        <v>2.4390243902439025E-2</v>
+      <c r="I47" s="86">
+        <v>1</v>
+      </c>
+      <c r="J47" s="86">
+        <v>1</v>
+      </c>
+      <c r="K47" s="81">
+        <v>1</v>
       </c>
       <c r="L47" s="5">
         <v>40</v>
@@ -3630,17 +3612,17 @@
       <c r="G48" s="5">
         <v>70752</v>
       </c>
-      <c r="H48" s="11">
+      <c r="H48" s="80">
         <v>1841</v>
       </c>
-      <c r="I48" s="13">
+      <c r="I48" s="86">
         <v>2.6020465852555404E-2</v>
       </c>
-      <c r="J48" s="13">
+      <c r="J48" s="86">
         <v>0.36820000000000003</v>
       </c>
-      <c r="K48" s="61">
-        <v>0.5</v>
+      <c r="K48" s="81">
+        <v>1</v>
       </c>
       <c r="L48" s="5">
         <v>70752</v>
@@ -3680,16 +3662,16 @@
       <c r="G49" s="5">
         <v>1776</v>
       </c>
-      <c r="H49" s="11">
+      <c r="H49" s="80">
         <v>1775</v>
       </c>
-      <c r="I49" s="13">
+      <c r="I49" s="86">
         <v>0.99943693693693691</v>
       </c>
-      <c r="J49" s="13">
+      <c r="J49" s="86">
         <v>0.99943693693693691</v>
       </c>
-      <c r="K49" s="61">
+      <c r="K49" s="81">
         <v>1</v>
       </c>
       <c r="L49" s="5">
@@ -3730,17 +3712,17 @@
       <c r="G50" s="5">
         <v>9902</v>
       </c>
-      <c r="H50" s="11">
-        <v>3540</v>
-      </c>
-      <c r="I50" s="13">
-        <v>0.35750353463946677</v>
-      </c>
-      <c r="J50" s="13">
-        <v>0.70799999999999996</v>
-      </c>
-      <c r="K50" s="61">
-        <v>0.16666666666666666</v>
+      <c r="H50" s="80">
+        <v>3515</v>
+      </c>
+      <c r="I50" s="86">
+        <v>0.35497879216319933</v>
+      </c>
+      <c r="J50" s="86">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="K50" s="81">
+        <v>0.2</v>
       </c>
       <c r="L50" s="5">
         <v>9902</v>
@@ -3780,16 +3762,16 @@
       <c r="G51" s="5">
         <v>5365</v>
       </c>
-      <c r="H51" s="11">
-        <v>1526</v>
-      </c>
-      <c r="I51" s="13">
-        <v>0.28443616029822927</v>
-      </c>
-      <c r="J51" s="13">
-        <v>0.30520000000000003</v>
-      </c>
-      <c r="K51" s="61">
+      <c r="H51" s="80">
+        <v>1625</v>
+      </c>
+      <c r="I51" s="86">
+        <v>0.30288909599254427</v>
+      </c>
+      <c r="J51" s="86">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="K51" s="81">
         <v>1</v>
       </c>
       <c r="L51" s="5">
@@ -3830,17 +3812,17 @@
       <c r="G52" s="5">
         <v>7322</v>
       </c>
-      <c r="H52" s="11">
-        <v>63</v>
-      </c>
-      <c r="I52" s="13">
-        <v>8.6042065009560229E-3</v>
-      </c>
-      <c r="J52" s="13">
-        <v>1.26E-2</v>
-      </c>
-      <c r="K52" s="61">
-        <v>2.2935779816513763E-3</v>
+      <c r="H52" s="80">
+        <v>201</v>
+      </c>
+      <c r="I52" s="86">
+        <v>2.7451515979240646E-2</v>
+      </c>
+      <c r="J52" s="86">
+        <v>4.02E-2</v>
+      </c>
+      <c r="K52" s="81">
+        <v>0.14285714285714285</v>
       </c>
       <c r="L52" s="5">
         <v>7322</v>
@@ -3880,17 +3862,17 @@
       <c r="G53" s="5">
         <v>760</v>
       </c>
-      <c r="H53" s="11">
-        <v>270</v>
-      </c>
-      <c r="I53" s="13">
-        <v>0.35526315789473684</v>
-      </c>
-      <c r="J53" s="13">
-        <v>0.35526315789473684</v>
-      </c>
-      <c r="K53" s="61">
-        <v>4.329004329004329E-3</v>
+      <c r="H53" s="80">
+        <v>7</v>
+      </c>
+      <c r="I53" s="86">
+        <v>9.2105263157894728E-3</v>
+      </c>
+      <c r="J53" s="86">
+        <v>9.2105263157894728E-3</v>
+      </c>
+      <c r="K53" s="81">
+        <v>9.7465886939571145E-4</v>
       </c>
       <c r="L53" s="5">
         <v>760</v>
@@ -3930,17 +3912,17 @@
       <c r="G54" s="5">
         <v>2379</v>
       </c>
-      <c r="H54" s="11">
-        <v>1396</v>
-      </c>
-      <c r="I54" s="13">
-        <v>0.58680117696511136</v>
-      </c>
-      <c r="J54" s="13">
-        <v>0.58680117696511136</v>
-      </c>
-      <c r="K54" s="61">
-        <v>0.5</v>
+      <c r="H54" s="80">
+        <v>1395</v>
+      </c>
+      <c r="I54" s="86">
+        <v>0.58638083228247162</v>
+      </c>
+      <c r="J54" s="86">
+        <v>0.58638083228247162</v>
+      </c>
+      <c r="K54" s="81">
+        <v>1</v>
       </c>
       <c r="L54" s="5">
         <v>2379</v>
@@ -3980,17 +3962,17 @@
       <c r="G55" s="5">
         <v>5</v>
       </c>
-      <c r="H55" s="11">
+      <c r="H55" s="80">
         <v>5</v>
       </c>
-      <c r="I55" s="13">
-        <v>1</v>
-      </c>
-      <c r="J55" s="13">
-        <v>1</v>
-      </c>
-      <c r="K55" s="61">
-        <v>0.5</v>
+      <c r="I55" s="86">
+        <v>1</v>
+      </c>
+      <c r="J55" s="86">
+        <v>1</v>
+      </c>
+      <c r="K55" s="81">
+        <v>0.25</v>
       </c>
       <c r="L55" s="5">
         <v>5</v>
@@ -4030,17 +4012,17 @@
       <c r="G56" s="5">
         <v>7</v>
       </c>
-      <c r="H56" s="11">
+      <c r="H56" s="80">
         <v>7</v>
       </c>
-      <c r="I56" s="13">
-        <v>1</v>
-      </c>
-      <c r="J56" s="13">
-        <v>1</v>
-      </c>
-      <c r="K56" s="61">
-        <v>1</v>
+      <c r="I56" s="86">
+        <v>1</v>
+      </c>
+      <c r="J56" s="86">
+        <v>1</v>
+      </c>
+      <c r="K56" s="81">
+        <v>0.33333333333333331</v>
       </c>
       <c r="L56" s="5">
         <v>7</v>
@@ -4080,16 +4062,16 @@
       <c r="G57" s="5">
         <v>859</v>
       </c>
-      <c r="H57" s="11">
-        <v>606</v>
-      </c>
-      <c r="I57" s="13">
-        <v>0.70547147846332947</v>
-      </c>
-      <c r="J57" s="13">
-        <v>0.70547147846332947</v>
-      </c>
-      <c r="K57" s="61">
+      <c r="H57" s="80">
+        <v>641</v>
+      </c>
+      <c r="I57" s="86">
+        <v>0.74621653084982542</v>
+      </c>
+      <c r="J57" s="86">
+        <v>0.74621653084982542</v>
+      </c>
+      <c r="K57" s="81">
         <v>0.5</v>
       </c>
       <c r="L57" s="5">
@@ -4130,17 +4112,17 @@
       <c r="G58" s="5">
         <v>4043</v>
       </c>
-      <c r="H58" s="11">
-        <v>613</v>
-      </c>
-      <c r="I58" s="13">
-        <v>0.15162008409596833</v>
-      </c>
-      <c r="J58" s="13">
-        <v>0.15162008409596833</v>
-      </c>
-      <c r="K58" s="61">
-        <v>1</v>
+      <c r="H58" s="80">
+        <v>2885</v>
+      </c>
+      <c r="I58" s="86">
+        <v>0.71357902547613161</v>
+      </c>
+      <c r="J58" s="86">
+        <v>0.71357902547613161</v>
+      </c>
+      <c r="K58" s="81">
+        <v>0.25</v>
       </c>
       <c r="L58" s="5">
         <v>4043</v>
@@ -4180,17 +4162,17 @@
       <c r="G59" s="5">
         <v>11</v>
       </c>
-      <c r="H59" s="11">
+      <c r="H59" s="80">
         <v>10</v>
       </c>
-      <c r="I59" s="13">
+      <c r="I59" s="86">
         <v>0.90909090909090906</v>
       </c>
-      <c r="J59" s="13">
+      <c r="J59" s="86">
         <v>0.90909090909090906</v>
       </c>
-      <c r="K59" s="61">
-        <v>0.04</v>
+      <c r="K59" s="81">
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="L59" s="5">
         <v>11</v>
@@ -4230,17 +4212,17 @@
       <c r="G60" s="5">
         <v>670</v>
       </c>
-      <c r="H60" s="11">
-        <v>52</v>
-      </c>
-      <c r="I60" s="13">
-        <v>7.7611940298507459E-2</v>
-      </c>
-      <c r="J60" s="13">
-        <v>7.7611940298507459E-2</v>
-      </c>
-      <c r="K60" s="61">
-        <v>4.7619047619047616E-2</v>
+      <c r="H60" s="80">
+        <v>64</v>
+      </c>
+      <c r="I60" s="86">
+        <v>9.5522388059701493E-2</v>
+      </c>
+      <c r="J60" s="86">
+        <v>9.5522388059701493E-2</v>
+      </c>
+      <c r="K60" s="81">
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="L60" s="5">
         <v>670</v>
@@ -4280,17 +4262,17 @@
       <c r="G61" s="5">
         <v>21</v>
       </c>
-      <c r="H61" s="11">
+      <c r="H61" s="80">
         <v>13</v>
       </c>
-      <c r="I61" s="13">
+      <c r="I61" s="86">
         <v>0.61904761904761907</v>
       </c>
-      <c r="J61" s="13">
+      <c r="J61" s="86">
         <v>0.61904761904761907</v>
       </c>
-      <c r="K61" s="61">
-        <v>0.1</v>
+      <c r="K61" s="81">
+        <v>0.2</v>
       </c>
       <c r="L61" s="5">
         <v>21</v>
@@ -4330,17 +4312,17 @@
       <c r="G62" s="5">
         <v>2</v>
       </c>
-      <c r="H62" s="11">
+      <c r="H62" s="80">
         <v>2</v>
       </c>
-      <c r="I62" s="13">
-        <v>1</v>
-      </c>
-      <c r="J62" s="13">
-        <v>1</v>
-      </c>
-      <c r="K62" s="61">
-        <v>5.8823529411764705E-2</v>
+      <c r="I62" s="86">
+        <v>1</v>
+      </c>
+      <c r="J62" s="86">
+        <v>1</v>
+      </c>
+      <c r="K62" s="81">
+        <v>0.1</v>
       </c>
       <c r="L62" s="5">
         <v>2</v>
@@ -4380,16 +4362,16 @@
       <c r="G63" s="5">
         <v>38</v>
       </c>
-      <c r="H63" s="11">
+      <c r="H63" s="80">
         <v>5</v>
       </c>
-      <c r="I63" s="13">
+      <c r="I63" s="86">
         <v>0.13157894736842105</v>
       </c>
-      <c r="J63" s="13">
+      <c r="J63" s="86">
         <v>0.13157894736842105</v>
       </c>
-      <c r="K63" s="61">
+      <c r="K63" s="81">
         <v>0.5</v>
       </c>
       <c r="L63" s="5">
@@ -4430,16 +4412,16 @@
       <c r="G64" s="5">
         <v>34</v>
       </c>
-      <c r="H64" s="11">
+      <c r="H64" s="80">
         <v>5</v>
       </c>
-      <c r="I64" s="13">
+      <c r="I64" s="86">
         <v>0.14705882352941177</v>
       </c>
-      <c r="J64" s="13">
+      <c r="J64" s="86">
         <v>0.14705882352941177</v>
       </c>
-      <c r="K64" s="61">
+      <c r="K64" s="81">
         <v>0.5</v>
       </c>
       <c r="L64" s="5">
@@ -4480,17 +4462,17 @@
       <c r="G65" s="5">
         <v>4</v>
       </c>
-      <c r="H65" s="11">
-        <v>1</v>
-      </c>
-      <c r="I65" s="13">
+      <c r="H65" s="80">
+        <v>1</v>
+      </c>
+      <c r="I65" s="86">
         <v>0.25</v>
       </c>
-      <c r="J65" s="13">
+      <c r="J65" s="86">
         <v>0.25</v>
       </c>
-      <c r="K65" s="61">
-        <v>1.1834319526627219E-3</v>
+      <c r="K65" s="81">
+        <v>1.3477088948787063E-3</v>
       </c>
       <c r="L65" s="5">
         <v>4</v>
@@ -4530,17 +4512,17 @@
       <c r="G66" s="5">
         <v>5</v>
       </c>
-      <c r="H66" s="11">
+      <c r="H66" s="80">
         <v>5</v>
       </c>
-      <c r="I66" s="13">
-        <v>1</v>
-      </c>
-      <c r="J66" s="13">
-        <v>1</v>
-      </c>
-      <c r="K66" s="61">
-        <v>0.2</v>
+      <c r="I66" s="86">
+        <v>1</v>
+      </c>
+      <c r="J66" s="86">
+        <v>1</v>
+      </c>
+      <c r="K66" s="81">
+        <v>0.16666666666666666</v>
       </c>
       <c r="L66" s="5">
         <v>5</v>
@@ -4580,17 +4562,17 @@
       <c r="G67" s="5">
         <v>1</v>
       </c>
-      <c r="H67" s="11">
-        <v>1</v>
-      </c>
-      <c r="I67" s="13">
-        <v>1</v>
-      </c>
-      <c r="J67" s="13">
-        <v>1</v>
-      </c>
-      <c r="K67" s="61">
-        <v>0.33333333333333331</v>
+      <c r="H67" s="80">
+        <v>1</v>
+      </c>
+      <c r="I67" s="86">
+        <v>1</v>
+      </c>
+      <c r="J67" s="86">
+        <v>1</v>
+      </c>
+      <c r="K67" s="81">
+        <v>0.25</v>
       </c>
       <c r="L67" s="5">
         <v>1</v>
@@ -4630,17 +4612,17 @@
       <c r="G68" s="5">
         <v>89</v>
       </c>
-      <c r="H68" s="11">
-        <v>38</v>
-      </c>
-      <c r="I68" s="13">
-        <v>0.42696629213483145</v>
-      </c>
-      <c r="J68" s="13">
-        <v>0.42696629213483145</v>
-      </c>
-      <c r="K68" s="61">
-        <v>7.6923076923076927E-2</v>
+      <c r="H68" s="80">
+        <v>51</v>
+      </c>
+      <c r="I68" s="86">
+        <v>0.5730337078651685</v>
+      </c>
+      <c r="J68" s="86">
+        <v>0.5730337078651685</v>
+      </c>
+      <c r="K68" s="81">
+        <v>6.25E-2</v>
       </c>
       <c r="L68" s="5">
         <v>89</v>
@@ -4680,16 +4662,16 @@
       <c r="G69" s="5">
         <v>290</v>
       </c>
-      <c r="H69" s="11">
-        <v>76</v>
-      </c>
-      <c r="I69" s="13">
-        <v>0.2620689655172414</v>
-      </c>
-      <c r="J69" s="13">
-        <v>0.2620689655172414</v>
-      </c>
-      <c r="K69" s="61">
+      <c r="H69" s="80">
+        <v>80</v>
+      </c>
+      <c r="I69" s="86">
+        <v>0.27586206896551724</v>
+      </c>
+      <c r="J69" s="86">
+        <v>0.27586206896551724</v>
+      </c>
+      <c r="K69" s="81">
         <v>0.14285714285714285</v>
       </c>
       <c r="L69" s="5">
@@ -4730,17 +4712,17 @@
       <c r="G70" s="5">
         <v>3</v>
       </c>
-      <c r="H70" s="11">
+      <c r="H70" s="80">
         <v>3</v>
       </c>
-      <c r="I70" s="13">
-        <v>1</v>
-      </c>
-      <c r="J70" s="13">
-        <v>1</v>
-      </c>
-      <c r="K70" s="61">
-        <v>0.1111111111111111</v>
+      <c r="I70" s="86">
+        <v>1</v>
+      </c>
+      <c r="J70" s="86">
+        <v>1</v>
+      </c>
+      <c r="K70" s="81">
+        <v>0.1</v>
       </c>
       <c r="L70" s="5">
         <v>3</v>
@@ -4780,16 +4762,16 @@
       <c r="G71" s="5">
         <v>2955</v>
       </c>
-      <c r="H71" s="11">
-        <v>3</v>
-      </c>
-      <c r="I71" s="13">
-        <v>1.0152284263959391E-3</v>
-      </c>
-      <c r="J71" s="13">
-        <v>1.0152284263959391E-3</v>
-      </c>
-      <c r="K71" s="61">
+      <c r="H71" s="80">
+        <v>457</v>
+      </c>
+      <c r="I71" s="86">
+        <v>0.15465313028764804</v>
+      </c>
+      <c r="J71" s="86">
+        <v>0.15465313028764804</v>
+      </c>
+      <c r="K71" s="81">
         <v>1</v>
       </c>
       <c r="L71" s="5">
@@ -4830,17 +4812,17 @@
       <c r="G72" s="5">
         <v>554</v>
       </c>
-      <c r="H72" s="11">
-        <v>6</v>
-      </c>
-      <c r="I72" s="13">
-        <v>1.0830324909747292E-2</v>
-      </c>
-      <c r="J72" s="13">
-        <v>1.0830324909747292E-2</v>
-      </c>
-      <c r="K72" s="61">
-        <v>0.33333333333333331</v>
+      <c r="H72" s="80">
+        <v>499</v>
+      </c>
+      <c r="I72" s="86">
+        <v>0.90072202166064985</v>
+      </c>
+      <c r="J72" s="86">
+        <v>0.90072202166064985</v>
+      </c>
+      <c r="K72" s="81">
+        <v>0.5</v>
       </c>
       <c r="L72" s="5">
         <v>554</v>
@@ -4880,17 +4862,17 @@
       <c r="G73" s="5">
         <v>5</v>
       </c>
-      <c r="H73" s="11">
+      <c r="H73" s="80">
         <v>2</v>
       </c>
-      <c r="I73" s="13">
+      <c r="I73" s="86">
         <v>0.4</v>
       </c>
-      <c r="J73" s="13">
+      <c r="J73" s="86">
         <v>0.4</v>
       </c>
-      <c r="K73" s="61">
-        <v>0.33333333333333331</v>
+      <c r="K73" s="81">
+        <v>0.125</v>
       </c>
       <c r="L73" s="5">
         <v>5</v>
@@ -4930,17 +4912,17 @@
       <c r="G74" s="5">
         <v>1003</v>
       </c>
-      <c r="H74" s="11">
-        <v>1</v>
-      </c>
-      <c r="I74" s="13">
-        <v>9.9700897308075765E-4</v>
-      </c>
-      <c r="J74" s="13">
-        <v>9.9700897308075765E-4</v>
-      </c>
-      <c r="K74" s="61">
-        <v>3.8910505836575876E-3</v>
+      <c r="H74" s="80">
+        <v>3</v>
+      </c>
+      <c r="I74" s="86">
+        <v>2.9910269192422734E-3</v>
+      </c>
+      <c r="J74" s="86">
+        <v>2.9910269192422734E-3</v>
+      </c>
+      <c r="K74" s="81">
+        <v>2.1008403361344537E-3</v>
       </c>
       <c r="L74" s="5">
         <v>1003</v>
@@ -4980,16 +4962,16 @@
       <c r="G75" s="5">
         <v>95</v>
       </c>
-      <c r="H75" s="11">
-        <v>0</v>
-      </c>
-      <c r="I75" s="13">
-        <v>0</v>
-      </c>
-      <c r="J75" s="13">
-        <v>0</v>
-      </c>
-      <c r="K75" s="61">
+      <c r="H75" s="80">
+        <v>0</v>
+      </c>
+      <c r="I75" s="86">
+        <v>0</v>
+      </c>
+      <c r="J75" s="86">
+        <v>0</v>
+      </c>
+      <c r="K75" s="81">
         <v>0</v>
       </c>
       <c r="L75" s="5">
@@ -5030,16 +5012,16 @@
       <c r="G76" s="5">
         <v>5</v>
       </c>
-      <c r="H76" s="11">
+      <c r="H76" s="80">
         <v>5</v>
       </c>
-      <c r="I76" s="13">
-        <v>1</v>
-      </c>
-      <c r="J76" s="13">
-        <v>1</v>
-      </c>
-      <c r="K76" s="61">
+      <c r="I76" s="86">
+        <v>1</v>
+      </c>
+      <c r="J76" s="86">
+        <v>1</v>
+      </c>
+      <c r="K76" s="81">
         <v>1</v>
       </c>
       <c r="L76" s="5">
@@ -5080,17 +5062,17 @@
       <c r="G77" s="5">
         <v>4079</v>
       </c>
-      <c r="H77" s="11">
-        <v>82</v>
-      </c>
-      <c r="I77" s="13">
-        <v>2.0102966413336601E-2</v>
-      </c>
-      <c r="J77" s="13">
-        <v>2.0102966413336601E-2</v>
-      </c>
-      <c r="K77" s="61">
-        <v>0.25</v>
+      <c r="H77" s="80">
+        <v>11</v>
+      </c>
+      <c r="I77" s="86">
+        <v>2.6967393969110076E-3</v>
+      </c>
+      <c r="J77" s="86">
+        <v>2.6967393969110076E-3</v>
+      </c>
+      <c r="K77" s="81">
+        <v>1.8867924528301886E-2</v>
       </c>
       <c r="L77" s="5">
         <v>4079</v>
@@ -5130,17 +5112,17 @@
       <c r="G78" s="5">
         <v>50</v>
       </c>
-      <c r="H78" s="11">
-        <v>35</v>
-      </c>
-      <c r="I78" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="J78" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="K78" s="61">
-        <v>1.4492753623188406E-2</v>
+      <c r="H78" s="80">
+        <v>34</v>
+      </c>
+      <c r="I78" s="86">
+        <v>0.68</v>
+      </c>
+      <c r="J78" s="86">
+        <v>0.68</v>
+      </c>
+      <c r="K78" s="81">
+        <v>1.2048192771084338E-2</v>
       </c>
       <c r="L78" s="5">
         <v>50</v>
@@ -5180,17 +5162,17 @@
       <c r="G79" s="5">
         <v>2505</v>
       </c>
-      <c r="H79" s="11">
-        <v>0</v>
-      </c>
-      <c r="I79" s="13">
-        <v>0</v>
-      </c>
-      <c r="J79" s="13">
-        <v>0</v>
-      </c>
-      <c r="K79" s="61">
-        <v>0</v>
+      <c r="H79" s="80">
+        <v>6</v>
+      </c>
+      <c r="I79" s="86">
+        <v>2.3952095808383233E-3</v>
+      </c>
+      <c r="J79" s="86">
+        <v>2.3952095808383233E-3</v>
+      </c>
+      <c r="K79" s="81">
+        <v>1.6393442622950821E-2</v>
       </c>
       <c r="L79" s="5">
         <v>2505</v>
@@ -5230,17 +5212,17 @@
       <c r="G80" s="5">
         <v>3</v>
       </c>
-      <c r="H80" s="11">
+      <c r="H80" s="80">
         <v>2</v>
       </c>
-      <c r="I80" s="13">
+      <c r="I80" s="86">
         <v>0.66666666666666663</v>
       </c>
-      <c r="J80" s="13">
+      <c r="J80" s="86">
         <v>0.66666666666666663</v>
       </c>
-      <c r="K80" s="61">
-        <v>4.5248868778280547E-3</v>
+      <c r="K80" s="81">
+        <v>1.838235294117647E-3</v>
       </c>
       <c r="L80" s="5">
         <v>3</v>
@@ -5280,16 +5262,16 @@
       <c r="G81" s="5">
         <v>13</v>
       </c>
-      <c r="H81" s="11">
-        <v>0</v>
-      </c>
-      <c r="I81" s="13">
-        <v>0</v>
-      </c>
-      <c r="J81" s="13">
-        <v>0</v>
-      </c>
-      <c r="K81" s="61">
+      <c r="H81" s="80">
+        <v>0</v>
+      </c>
+      <c r="I81" s="86">
+        <v>0</v>
+      </c>
+      <c r="J81" s="86">
+        <v>0</v>
+      </c>
+      <c r="K81" s="81">
         <v>0</v>
       </c>
       <c r="L81" s="5">
@@ -5330,17 +5312,17 @@
       <c r="G82" s="5">
         <v>1763</v>
       </c>
-      <c r="H82" s="11">
-        <v>5</v>
-      </c>
-      <c r="I82" s="13">
-        <v>2.8360748723766306E-3</v>
-      </c>
-      <c r="J82" s="13">
-        <v>2.8360748723766306E-3</v>
-      </c>
-      <c r="K82" s="61">
-        <v>6.5445026178010475E-4</v>
+      <c r="H82" s="80">
+        <v>20</v>
+      </c>
+      <c r="I82" s="86">
+        <v>1.1344299489506523E-2</v>
+      </c>
+      <c r="J82" s="86">
+        <v>1.1344299489506523E-2</v>
+      </c>
+      <c r="K82" s="81">
+        <v>1.1363636363636364E-2</v>
       </c>
       <c r="L82" s="5">
         <v>1763</v>
@@ -5380,17 +5362,17 @@
       <c r="G83" s="5">
         <v>2917</v>
       </c>
-      <c r="H83" s="11">
-        <v>84</v>
-      </c>
-      <c r="I83" s="15">
-        <v>2.8796708947548853E-2</v>
-      </c>
-      <c r="J83" s="13">
-        <v>2.8796708947548853E-2</v>
-      </c>
-      <c r="K83" s="61">
-        <v>3.5971223021582736E-3</v>
+      <c r="H83" s="80">
+        <v>96</v>
+      </c>
+      <c r="I83" s="87">
+        <v>3.29105245114844E-2</v>
+      </c>
+      <c r="J83" s="86">
+        <v>3.29105245114844E-2</v>
+      </c>
+      <c r="K83" s="81">
+        <v>6.6225165562913907E-3</v>
       </c>
       <c r="L83" s="5">
         <v>2917</v>
@@ -5438,19 +5420,19 @@
       </c>
       <c r="H84" s="16">
         <f>SUM(H14:H83)</f>
-        <v>19718</v>
+        <v>21933</v>
       </c>
       <c r="I84" s="119">
         <f t="shared" ref="I84:K84" si="1">AVERAGE(I14:I83)</f>
-        <v>0.44698303878847329</v>
+        <v>0.43962918757624037</v>
       </c>
       <c r="J84" s="119">
         <f t="shared" si="1"/>
-        <v>0.47177225746794005</v>
+        <v>0.46365583873452254</v>
       </c>
       <c r="K84" s="62">
         <f t="shared" si="1"/>
-        <v>0.31066038932423218</v>
+        <v>0.3173935812924561</v>
       </c>
       <c r="L84" s="37">
         <f>SUM(L14:L83)</f>
@@ -5532,7 +5514,7 @@
       </c>
       <c r="B93" s="74">
         <f>I84</f>
-        <v>0.44698303878847329</v>
+        <v>0.43962918757624037</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
@@ -5541,7 +5523,7 @@
       </c>
       <c r="B94" s="74">
         <f>J84</f>
-        <v>0.47177225746794005</v>
+        <v>0.46365583873452254</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
@@ -5550,7 +5532,7 @@
       </c>
       <c r="B95" s="78">
         <f>K84</f>
-        <v>0.31066038932423218</v>
+        <v>0.3173935812924561</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -9906,17 +9888,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14 I14">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>"I14&gt;D14"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>"I16&gt;D16"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>"I16&gt;D16"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9985,8 +9967,8 @@
   </sheetPr>
   <dimension ref="A1:P104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:K4"/>
+    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O87" sqref="O87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10417,16 +10399,16 @@
         <v>9</v>
       </c>
       <c r="M14" s="50">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="N14" s="51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O14" s="52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14" s="64">
-        <v>0</v>
+        <v>5.3191489361702126E-3</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -10467,16 +10449,16 @@
         <v>1160</v>
       </c>
       <c r="M15" s="50">
-        <v>727</v>
+        <v>299</v>
       </c>
       <c r="N15" s="52">
-        <v>0.62672413793103443</v>
+        <v>0.25775862068965516</v>
       </c>
       <c r="O15" s="52">
-        <v>0.62672413793103443</v>
+        <v>0.25775862068965516</v>
       </c>
       <c r="P15" s="64">
-        <v>3.125E-2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -10517,16 +10499,16 @@
         <v>1554</v>
       </c>
       <c r="M16" s="50">
-        <v>760</v>
+        <v>0</v>
       </c>
       <c r="N16" s="52">
-        <v>0.48906048906048905</v>
+        <v>0</v>
       </c>
       <c r="O16" s="52">
-        <v>0.48906048906048905</v>
+        <v>0</v>
       </c>
       <c r="P16" s="64">
-        <v>0.14285714285714285</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -10567,16 +10549,16 @@
         <v>28</v>
       </c>
       <c r="M17" s="50">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="N17" s="52">
-        <v>3.5714285714285712E-2</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="O17" s="52">
-        <v>3.5714285714285712E-2</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="P17" s="64">
-        <v>1</v>
+        <v>9.9009900990099011E-3</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -10617,16 +10599,16 @@
         <v>553</v>
       </c>
       <c r="M18" s="50">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="N18" s="52">
-        <v>8.3182640144665462E-2</v>
+        <v>0.23869801084990958</v>
       </c>
       <c r="O18" s="52">
-        <v>8.3182640144665462E-2</v>
+        <v>0.23869801084990958</v>
       </c>
       <c r="P18" s="64">
-        <v>8.0645161290322578E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -10667,16 +10649,16 @@
         <v>431</v>
       </c>
       <c r="M19" s="50">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="N19" s="52">
-        <v>6.9605568445475635E-2</v>
+        <v>3.4802784222737818E-2</v>
       </c>
       <c r="O19" s="52">
-        <v>6.9605568445475635E-2</v>
+        <v>3.4802784222737818E-2</v>
       </c>
       <c r="P19" s="64">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -10717,16 +10699,16 @@
         <v>97768</v>
       </c>
       <c r="M20" s="50">
-        <v>1552</v>
+        <v>256</v>
       </c>
       <c r="N20" s="52">
-        <v>1.5874314704197694E-2</v>
+        <v>2.6184436625480731E-3</v>
       </c>
       <c r="O20" s="52">
-        <v>0.31040000000000001</v>
+        <v>5.1200000000000002E-2</v>
       </c>
       <c r="P20" s="64">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -10776,7 +10758,7 @@
         <v>0.9642857142857143</v>
       </c>
       <c r="P21" s="64">
-        <v>1.321003963011889E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -10817,16 +10799,16 @@
         <v>1554</v>
       </c>
       <c r="M22" s="50">
-        <v>58</v>
+        <v>710</v>
       </c>
       <c r="N22" s="52">
-        <v>3.7323037323037322E-2</v>
+        <v>0.4568854568854569</v>
       </c>
       <c r="O22" s="52">
-        <v>3.7323037323037322E-2</v>
+        <v>0.4568854568854569</v>
       </c>
       <c r="P22" s="64">
-        <v>1.8552875695732839E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -10867,16 +10849,16 @@
         <v>123</v>
       </c>
       <c r="M23" s="50">
-        <v>122</v>
+        <v>0</v>
       </c>
       <c r="N23" s="52">
-        <v>0.99186991869918695</v>
+        <v>0</v>
       </c>
       <c r="O23" s="52">
-        <v>0.99186991869918695</v>
+        <v>0</v>
       </c>
       <c r="P23" s="64">
-        <v>3.6900369003690036E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -10917,16 +10899,16 @@
         <v>40485</v>
       </c>
       <c r="M24" s="50">
-        <v>3904</v>
+        <v>0</v>
       </c>
       <c r="N24" s="52">
-        <v>9.6430776830925033E-2</v>
+        <v>0</v>
       </c>
       <c r="O24" s="52">
-        <v>0.78080000000000005</v>
+        <v>0</v>
       </c>
       <c r="P24" s="64">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -10967,16 +10949,16 @@
         <v>388</v>
       </c>
       <c r="M25" s="50">
-        <v>310</v>
+        <v>252</v>
       </c>
       <c r="N25" s="52">
-        <v>0.7989690721649485</v>
+        <v>0.64948453608247425</v>
       </c>
       <c r="O25" s="52">
-        <v>0.7989690721649485</v>
+        <v>0.64948453608247425</v>
       </c>
       <c r="P25" s="64">
-        <v>4.3103448275862068E-3</v>
+        <v>2.0408163265306121E-2</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -11017,16 +10999,16 @@
         <v>577</v>
       </c>
       <c r="M26" s="50">
-        <v>539</v>
+        <v>103</v>
       </c>
       <c r="N26" s="52">
-        <v>0.9341421143847487</v>
+        <v>0.17850953206239167</v>
       </c>
       <c r="O26" s="52">
-        <v>0.9341421143847487</v>
+        <v>0.17850953206239167</v>
       </c>
       <c r="P26" s="64">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -11067,16 +11049,16 @@
         <v>142</v>
       </c>
       <c r="M27" s="50">
-        <v>6</v>
+        <v>123</v>
       </c>
       <c r="N27" s="52">
-        <v>4.2253521126760563E-2</v>
+        <v>0.86619718309859151</v>
       </c>
       <c r="O27" s="52">
-        <v>4.2253521126760563E-2</v>
+        <v>0.86619718309859151</v>
       </c>
       <c r="P27" s="64">
-        <v>5.3966540744738263E-4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -11117,13 +11099,13 @@
         <v>158355</v>
       </c>
       <c r="M28" s="50">
-        <v>4868</v>
+        <v>33252</v>
       </c>
       <c r="N28" s="52">
-        <v>3.0741056487007042E-2</v>
+        <v>0.20998389694041869</v>
       </c>
       <c r="O28" s="52">
-        <v>0.97360000000000002</v>
+        <v>0.9983786705098181</v>
       </c>
       <c r="P28" s="64">
         <v>1</v>
@@ -11167,13 +11149,13 @@
         <v>323</v>
       </c>
       <c r="M29" s="50">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="N29" s="52">
-        <v>0.9876160990712074</v>
+        <v>0.94117647058823528</v>
       </c>
       <c r="O29" s="52">
-        <v>0.9876160990712074</v>
+        <v>0.94117647058823528</v>
       </c>
       <c r="P29" s="64">
         <v>1</v>
@@ -11217,16 +11199,16 @@
         <v>5</v>
       </c>
       <c r="M30" s="50">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N30" s="52">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="O30" s="52">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="P30" s="64">
-        <v>1.1764705882352941E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -11267,13 +11249,13 @@
         <v>13</v>
       </c>
       <c r="M31" s="50">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="N31" s="52">
-        <v>1</v>
+        <v>0.61538461538461542</v>
       </c>
       <c r="O31" s="52">
-        <v>1</v>
+        <v>0.61538461538461542</v>
       </c>
       <c r="P31" s="64">
         <v>1</v>
@@ -11317,16 +11299,16 @@
         <v>158</v>
       </c>
       <c r="M32" s="50">
-        <v>149</v>
+        <v>98</v>
       </c>
       <c r="N32" s="52">
-        <v>0.94303797468354433</v>
+        <v>0.620253164556962</v>
       </c>
       <c r="O32" s="52">
-        <v>0.94303797468354433</v>
+        <v>0.620253164556962</v>
       </c>
       <c r="P32" s="64">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -11367,13 +11349,13 @@
         <v>247</v>
       </c>
       <c r="M33" s="50">
-        <v>226</v>
+        <v>1</v>
       </c>
       <c r="N33" s="52">
-        <v>0.91497975708502022</v>
+        <v>4.048582995951417E-3</v>
       </c>
       <c r="O33" s="52">
-        <v>0.91497975708502022</v>
+        <v>4.048582995951417E-3</v>
       </c>
       <c r="P33" s="64">
         <v>1</v>
@@ -11417,16 +11399,16 @@
         <v>83</v>
       </c>
       <c r="M34" s="50">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="N34" s="52">
-        <v>0.95180722891566261</v>
+        <v>0.86746987951807231</v>
       </c>
       <c r="O34" s="52">
-        <v>0.95180722891566261</v>
+        <v>0.86746987951807231</v>
       </c>
       <c r="P34" s="64">
-        <v>1.9047619047619048E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -11476,7 +11458,7 @@
         <v>1</v>
       </c>
       <c r="P35" s="64">
-        <v>6.1349693251533744E-3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -11517,16 +11499,16 @@
         <v>24</v>
       </c>
       <c r="M36" s="50">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="N36" s="52">
-        <v>0.625</v>
+        <v>0</v>
       </c>
       <c r="O36" s="52">
-        <v>0.625</v>
+        <v>0</v>
       </c>
       <c r="P36" s="64">
-        <v>5.2910052910052907E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -11567,16 +11549,16 @@
         <v>35</v>
       </c>
       <c r="M37" s="50">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="N37" s="52">
-        <v>0.62857142857142856</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="O37" s="52">
-        <v>0.62857142857142856</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="P37" s="64">
-        <v>4.96031746031746E-4</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -11617,16 +11599,16 @@
         <v>88</v>
       </c>
       <c r="M38" s="50">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="N38" s="52">
-        <v>0.32954545454545453</v>
+        <v>0</v>
       </c>
       <c r="O38" s="52">
-        <v>0.32954545454545453</v>
+        <v>0</v>
       </c>
       <c r="P38" s="64">
-        <v>1.0351966873706005E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -11667,16 +11649,16 @@
         <v>80</v>
       </c>
       <c r="M39" s="50">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="N39" s="52">
-        <v>0.65</v>
+        <v>0.61250000000000004</v>
       </c>
       <c r="O39" s="52">
-        <v>0.65</v>
+        <v>0.61250000000000004</v>
       </c>
       <c r="P39" s="64">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -11726,7 +11708,7 @@
         <v>0.80303030303030298</v>
       </c>
       <c r="P40" s="64">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -11767,16 +11749,16 @@
         <v>15</v>
       </c>
       <c r="M41" s="50">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="N41" s="52">
-        <v>0.73333333333333328</v>
+        <v>0</v>
       </c>
       <c r="O41" s="52">
-        <v>0.73333333333333328</v>
+        <v>0</v>
       </c>
       <c r="P41" s="64">
-        <v>3.7037037037037035E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -11817,13 +11799,13 @@
         <v>332</v>
       </c>
       <c r="M42" s="50">
-        <v>286</v>
+        <v>11</v>
       </c>
       <c r="N42" s="52">
-        <v>0.86144578313253017</v>
+        <v>3.313253012048193E-2</v>
       </c>
       <c r="O42" s="52">
-        <v>0.86144578313253017</v>
+        <v>3.313253012048193E-2</v>
       </c>
       <c r="P42" s="64">
         <v>1</v>
@@ -11867,16 +11849,16 @@
         <v>39</v>
       </c>
       <c r="M43" s="50">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="N43" s="52">
-        <v>0.74358974358974361</v>
+        <v>0.10256410256410256</v>
       </c>
       <c r="O43" s="52">
-        <v>0.74358974358974361</v>
+        <v>0.10256410256410256</v>
       </c>
       <c r="P43" s="64">
-        <v>0.05</v>
+        <v>3.3333333333333333E-2</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -11926,7 +11908,7 @@
         <v>1</v>
       </c>
       <c r="P44" s="64">
-        <v>4.391743522178305E-4</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -11967,16 +11949,16 @@
         <v>431</v>
       </c>
       <c r="M45" s="50">
-        <v>59</v>
+        <v>412</v>
       </c>
       <c r="N45" s="52">
-        <v>0.1368909512761021</v>
+        <v>0.95591647331786544</v>
       </c>
       <c r="O45" s="52">
-        <v>0.1368909512761021</v>
+        <v>0.95591647331786544</v>
       </c>
       <c r="P45" s="64">
-        <v>1.4513788098693759E-3</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -12017,16 +11999,16 @@
         <v>40</v>
       </c>
       <c r="M46" s="50">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="N46" s="52">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="O46" s="52">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="P46" s="64">
-        <v>8.3612040133779263E-4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -12067,16 +12049,16 @@
         <v>40</v>
       </c>
       <c r="M47" s="50">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="N47" s="52">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="O47" s="52">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="P47" s="64">
-        <v>4.0650406504065045E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -12117,13 +12099,13 @@
         <v>70752</v>
       </c>
       <c r="M48" s="50">
-        <v>482</v>
+        <v>1945</v>
       </c>
       <c r="N48" s="52">
-        <v>6.8125282677521486E-3</v>
+        <v>2.7490388964269561E-2</v>
       </c>
       <c r="O48" s="52">
-        <v>9.64E-2</v>
+        <v>0.38900000000000001</v>
       </c>
       <c r="P48" s="64">
         <v>1</v>
@@ -12167,13 +12149,13 @@
         <v>1776</v>
       </c>
       <c r="M49" s="50">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="N49" s="52">
-        <v>1</v>
+        <v>0.99943693693693691</v>
       </c>
       <c r="O49" s="52">
-        <v>1</v>
+        <v>0.99943693693693691</v>
       </c>
       <c r="P49" s="64">
         <v>1</v>
@@ -12217,16 +12199,16 @@
         <v>9902</v>
       </c>
       <c r="M50" s="50">
-        <v>2641</v>
+        <v>4837</v>
       </c>
       <c r="N50" s="52">
-        <v>0.26671379519289035</v>
+        <v>0.48848717430822058</v>
       </c>
       <c r="O50" s="52">
-        <v>0.5282</v>
+        <v>0.96740000000000004</v>
       </c>
       <c r="P50" s="64">
-        <v>1.7241379310344827E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -12267,16 +12249,16 @@
         <v>5365</v>
       </c>
       <c r="M51" s="50">
-        <v>1316</v>
+        <v>1876</v>
       </c>
       <c r="N51" s="52">
-        <v>0.24529356943150046</v>
+        <v>0.34967381174277729</v>
       </c>
       <c r="O51" s="52">
-        <v>0.26319999999999999</v>
+        <v>0.37519999999999998</v>
       </c>
       <c r="P51" s="64">
-        <v>0.5</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -12317,16 +12299,16 @@
         <v>7322</v>
       </c>
       <c r="M52" s="50">
-        <v>1503</v>
+        <v>104</v>
       </c>
       <c r="N52" s="52">
-        <v>0.20527178366566512</v>
+        <v>1.4203769461895657E-2</v>
       </c>
       <c r="O52" s="52">
-        <v>0.30059999999999998</v>
+        <v>2.0799999999999999E-2</v>
       </c>
       <c r="P52" s="64">
-        <v>0.5</v>
+        <v>5.3763440860215058E-3</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
@@ -12367,16 +12349,16 @@
         <v>760</v>
       </c>
       <c r="M53" s="50">
-        <v>666</v>
+        <v>760</v>
       </c>
       <c r="N53" s="52">
-        <v>0.87631578947368416</v>
+        <v>1</v>
       </c>
       <c r="O53" s="52">
-        <v>0.87631578947368416</v>
+        <v>1</v>
       </c>
       <c r="P53" s="64">
-        <v>1</v>
+        <v>3.2258064516129031E-2</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -12426,7 +12408,7 @@
         <v>1</v>
       </c>
       <c r="P54" s="64">
-        <v>1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -12476,7 +12458,7 @@
         <v>1</v>
       </c>
       <c r="P55" s="64">
-        <v>1.6501650165016502E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -12526,7 +12508,7 @@
         <v>1</v>
       </c>
       <c r="P56" s="64">
-        <v>1.0822510822510823E-3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -12567,16 +12549,16 @@
         <v>859</v>
       </c>
       <c r="M57" s="50">
-        <v>194</v>
+        <v>644</v>
       </c>
       <c r="N57" s="52">
-        <v>0.22584400465657742</v>
+        <v>0.74970896391152508</v>
       </c>
       <c r="O57" s="52">
-        <v>0.22584400465657742</v>
+        <v>0.74970896391152508</v>
       </c>
       <c r="P57" s="64">
-        <v>2.0408163265306121E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -12617,16 +12599,16 @@
         <v>4043</v>
       </c>
       <c r="M58" s="50">
-        <v>829</v>
+        <v>3005</v>
       </c>
       <c r="N58" s="52">
-        <v>0.20504575810042047</v>
+        <v>0.74325995547860502</v>
       </c>
       <c r="O58" s="52">
-        <v>0.20504575810042047</v>
+        <v>0.74325995547860502</v>
       </c>
       <c r="P58" s="64">
-        <v>2.2222222222222223E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -12676,7 +12658,7 @@
         <v>0.90909090909090906</v>
       </c>
       <c r="P59" s="64">
-        <v>3.1645569620253164E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
@@ -12717,16 +12699,16 @@
         <v>670</v>
       </c>
       <c r="M60" s="50">
-        <v>623</v>
+        <v>64</v>
       </c>
       <c r="N60" s="52">
-        <v>0.92985074626865671</v>
+        <v>9.5522388059701493E-2</v>
       </c>
       <c r="O60" s="52">
-        <v>0.92985074626865671</v>
+        <v>9.5522388059701493E-2</v>
       </c>
       <c r="P60" s="64">
-        <v>0.125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
@@ -12767,16 +12749,16 @@
         <v>21</v>
       </c>
       <c r="M61" s="50">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="N61" s="52">
-        <v>0.38095238095238093</v>
+        <v>0.61904761904761907</v>
       </c>
       <c r="O61" s="52">
-        <v>0.38095238095238093</v>
+        <v>0.61904761904761907</v>
       </c>
       <c r="P61" s="64">
-        <v>9.2421441774491681E-4</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
@@ -12817,16 +12799,16 @@
         <v>2</v>
       </c>
       <c r="M62" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N62" s="52">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O62" s="52">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P62" s="64">
-        <v>2.6560424966799468E-4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
@@ -12867,16 +12849,16 @@
         <v>38</v>
       </c>
       <c r="M63" s="50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N63" s="52">
-        <v>2.6315789473684209E-2</v>
+        <v>0</v>
       </c>
       <c r="O63" s="52">
-        <v>2.6315789473684209E-2</v>
+        <v>0</v>
       </c>
       <c r="P63" s="64">
-        <v>2.3696682464454978E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
@@ -12917,16 +12899,16 @@
         <v>34</v>
       </c>
       <c r="M64" s="50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N64" s="52">
-        <v>2.9411764705882353E-2</v>
+        <v>0</v>
       </c>
       <c r="O64" s="52">
-        <v>2.9411764705882353E-2</v>
+        <v>0</v>
       </c>
       <c r="P64" s="64">
-        <v>5.8823529411764705E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
@@ -12967,16 +12949,16 @@
         <v>4</v>
       </c>
       <c r="M65" s="50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N65" s="52">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="O65" s="52">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="P65" s="64">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
@@ -13026,7 +13008,7 @@
         <v>1</v>
       </c>
       <c r="P66" s="64">
-        <v>1.0752688172043012E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
@@ -13076,7 +13058,7 @@
         <v>1</v>
       </c>
       <c r="P67" s="64">
-        <v>5.4644808743169399E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
@@ -13117,16 +13099,16 @@
         <v>89</v>
       </c>
       <c r="M68" s="50">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="N68" s="52">
-        <v>1</v>
+        <v>0.6741573033707865</v>
       </c>
       <c r="O68" s="52">
-        <v>1</v>
+        <v>0.6741573033707865</v>
       </c>
       <c r="P68" s="64">
-        <v>2.2222222222222223E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
@@ -13167,16 +13149,16 @@
         <v>290</v>
       </c>
       <c r="M69" s="50">
-        <v>289</v>
+        <v>130</v>
       </c>
       <c r="N69" s="52">
-        <v>0.99655172413793103</v>
+        <v>0.44827586206896552</v>
       </c>
       <c r="O69" s="52">
-        <v>0.99655172413793103</v>
+        <v>0.44827586206896552</v>
       </c>
       <c r="P69" s="64">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
@@ -13226,7 +13208,7 @@
         <v>1</v>
       </c>
       <c r="P70" s="64">
-        <v>1.6949152542372881E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
@@ -13267,16 +13249,16 @@
         <v>2955</v>
       </c>
       <c r="M71" s="50">
-        <v>2770</v>
+        <v>573</v>
       </c>
       <c r="N71" s="52">
-        <v>0.93739424703891705</v>
+        <v>0.19390862944162437</v>
       </c>
       <c r="O71" s="52">
-        <v>0.93739424703891705</v>
+        <v>0.19390862944162437</v>
       </c>
       <c r="P71" s="64">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
@@ -13317,16 +13299,16 @@
         <v>554</v>
       </c>
       <c r="M72" s="50">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N72" s="52">
-        <v>1.0830324909747292E-2</v>
+        <v>9.0252707581227436E-3</v>
       </c>
       <c r="O72" s="52">
-        <v>1.0830324909747292E-2</v>
+        <v>9.0252707581227436E-3</v>
       </c>
       <c r="P72" s="64">
-        <v>2.4213075060532689E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
@@ -13367,16 +13349,16 @@
         <v>5</v>
       </c>
       <c r="M73" s="50">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N73" s="52">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="O73" s="52">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="P73" s="64">
-        <v>5.4975261132490382E-4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
@@ -13417,16 +13399,16 @@
         <v>1003</v>
       </c>
       <c r="M74" s="50">
-        <v>641</v>
+        <v>1</v>
       </c>
       <c r="N74" s="52">
-        <v>0.6390827517447657</v>
+        <v>9.9700897308075765E-4</v>
       </c>
       <c r="O74" s="52">
-        <v>0.6390827517447657</v>
+        <v>9.9700897308075765E-4</v>
       </c>
       <c r="P74" s="64">
-        <v>1</v>
+        <v>8.2644628099173556E-3</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
@@ -13467,16 +13449,16 @@
         <v>95</v>
       </c>
       <c r="M75" s="50">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="N75" s="52">
-        <v>0.50526315789473686</v>
+        <v>0</v>
       </c>
       <c r="O75" s="52">
-        <v>0.50526315789473686</v>
+        <v>0</v>
       </c>
       <c r="P75" s="64">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
@@ -13517,16 +13499,16 @@
         <v>5</v>
       </c>
       <c r="M76" s="50">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N76" s="52">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="O76" s="52">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="P76" s="64">
-        <v>3.1826861871419476E-4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
@@ -13567,13 +13549,13 @@
         <v>4079</v>
       </c>
       <c r="M77" s="50">
-        <v>411</v>
+        <v>20</v>
       </c>
       <c r="N77" s="52">
-        <v>0.10075999019367492</v>
+        <v>4.9031625398381958E-3</v>
       </c>
       <c r="O77" s="52">
-        <v>0.10075999019367492</v>
+        <v>4.9031625398381958E-3</v>
       </c>
       <c r="P77" s="64">
         <v>0.5</v>
@@ -13617,16 +13599,16 @@
         <v>50</v>
       </c>
       <c r="M78" s="50">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="N78" s="52">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="O78" s="52">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="P78" s="64">
-        <v>0</v>
+        <v>7.1428571428571425E-2</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
@@ -13667,16 +13649,16 @@
         <v>2505</v>
       </c>
       <c r="M79" s="50">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="N79" s="52">
-        <v>0</v>
+        <v>1.3572854291417165E-2</v>
       </c>
       <c r="O79" s="52">
-        <v>0</v>
+        <v>1.3572854291417165E-2</v>
       </c>
       <c r="P79" s="64">
-        <v>0</v>
+        <v>3.3333333333333333E-2</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -13717,16 +13699,16 @@
         <v>3</v>
       </c>
       <c r="M80" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N80" s="52">
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="O80" s="52">
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="P80" s="64">
-        <v>2.7247956403269754E-3</v>
+        <v>4.7619047619047616E-2</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
@@ -13767,16 +13749,16 @@
         <v>13</v>
       </c>
       <c r="M81" s="50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N81" s="52">
-        <v>7.6923076923076927E-2</v>
+        <v>0</v>
       </c>
       <c r="O81" s="52">
-        <v>7.6923076923076927E-2</v>
+        <v>0</v>
       </c>
       <c r="P81" s="64">
-        <v>5.6116722783389455E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
@@ -13817,16 +13799,16 @@
         <v>1763</v>
       </c>
       <c r="M82" s="50">
-        <v>156</v>
+        <v>354</v>
       </c>
       <c r="N82" s="52">
-        <v>8.8485536018150873E-2</v>
+        <v>0.20079410096426545</v>
       </c>
       <c r="O82" s="52">
-        <v>8.8485536018150873E-2</v>
+        <v>0.20079410096426545</v>
       </c>
       <c r="P82" s="64">
-        <v>0.125</v>
+        <v>6.6666666666666666E-2</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
@@ -13867,16 +13849,16 @@
         <v>2917</v>
       </c>
       <c r="M83" s="50">
-        <v>102</v>
+        <v>536</v>
       </c>
       <c r="N83" s="54">
-        <v>3.4967432293452179E-2</v>
+        <v>0.18375042852245457</v>
       </c>
       <c r="O83" s="52">
-        <v>3.4967432293452179E-2</v>
+        <v>0.18375042852245457</v>
       </c>
       <c r="P83" s="64">
-        <v>1.2048192771084338E-2</v>
+        <v>1.0604453870625664E-3</v>
       </c>
     </row>
     <row r="84" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13925,19 +13907,19 @@
       </c>
       <c r="M84" s="67">
         <f>SUM(M14:M83)</f>
-        <v>31358</v>
+        <v>55537</v>
       </c>
       <c r="N84" s="70">
         <f t="shared" ref="N84:P84" si="1">AVERAGE(N14:N83)</f>
-        <v>0.55115050140435129</v>
+        <v>0.48468717252692506</v>
       </c>
       <c r="O84" s="70">
         <f t="shared" si="1"/>
-        <v>0.58523710391035222</v>
+        <v>0.50910890374734907</v>
       </c>
       <c r="P84" s="57">
         <f t="shared" si="1"/>
-        <v>0.24190248383969909</v>
+        <v>0.55499359864019859</v>
       </c>
     </row>
     <row r="85" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -14067,11 +14049,6 @@
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="M10:N10"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="M8:N8"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="E7:F7"/>
@@ -14079,11 +14056,11 @@
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="O7:P7"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="M8:N8"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E5:F5"/>
@@ -14091,11 +14068,11 @@
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="O5:P5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="M6:N6"/>
     <mergeCell ref="O4:P4"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="H1:K1"/>
@@ -14106,6 +14083,11 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="O3:P3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="M4:N4"/>
   </mergeCells>
   <conditionalFormatting sqref="D14:F84">
     <cfRule type="dataBar" priority="6">
@@ -14136,17 +14118,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14 I14">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>"I14&gt;D14"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>"I16&gt;D16"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>"I16&gt;D16"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36398,8 +36380,8 @@
   </sheetPr>
   <dimension ref="A1:U104"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S84" sqref="S84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41793,8 +41775,8 @@
   </sheetPr>
   <dimension ref="A1:P104"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="N82" sqref="N82"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45627,7 +45609,7 @@
         <v>211</v>
       </c>
       <c r="N82" s="52">
-        <v>0.11968235961429381</v>
+        <v>0.11968235961429401</v>
       </c>
       <c r="O82" s="52">
         <v>0.11968235961429381</v>
@@ -45964,7 +45946,7 @@
   </sheetPr>
   <dimension ref="A1:K104"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K84" sqref="K84"/>
     </sheetView>
   </sheetViews>
@@ -54358,7 +54340,7 @@
   </sheetPr>
   <dimension ref="A1:K104"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
@@ -65615,17 +65597,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14 I14">
-    <cfRule type="expression" dxfId="11" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>"I14&gt;D14"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>"I16&gt;D16"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>"I16&gt;D16"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>